<commit_message>
intento dos de excel
</commit_message>
<xml_diff>
--- a/Libro.xlsx
+++ b/Libro.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26920"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6395387C-01F0-4D62-B03D-4F4654B5D5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\progra\PBN.23B.Equipo11\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5872A2A9-55F4-4761-A3D1-42A1ECB72D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>ETQ</t>
   </si>
@@ -52,6 +57,147 @@
   </si>
   <si>
     <t>END</t>
+  </si>
+  <si>
+    <t>Et1:</t>
+  </si>
+  <si>
+    <t>dos:</t>
+  </si>
+  <si>
+    <t>Tres:</t>
+  </si>
+  <si>
+    <t>SWI</t>
+  </si>
+  <si>
+    <t>EORA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@5 </t>
+  </si>
+  <si>
+    <t>%111</t>
+  </si>
+  <si>
+    <t>$FFF</t>
+  </si>
+  <si>
+    <t>#5</t>
+  </si>
+  <si>
+    <t>#@5</t>
+  </si>
+  <si>
+    <t>#1500</t>
+  </si>
+  <si>
+    <t>1,X</t>
+  </si>
+  <si>
+    <t>255,X</t>
+  </si>
+  <si>
+    <t>32768,X</t>
+  </si>
+  <si>
+    <t>1,+PC</t>
+  </si>
+  <si>
+    <t>A,X</t>
+  </si>
+  <si>
+    <t>254,X</t>
+  </si>
+  <si>
+    <t>64444,X</t>
+  </si>
+  <si>
+    <t>[1,X]</t>
+  </si>
+  <si>
+    <t>[6444,X]</t>
+  </si>
+  <si>
+    <t>[D,X]</t>
+  </si>
+  <si>
+    <t>UNO</t>
+  </si>
+  <si>
+    <t>A,UNO</t>
+  </si>
+  <si>
+    <t>BLT</t>
+  </si>
+  <si>
+    <t>LBLT</t>
+  </si>
+  <si>
+    <t>IBNE</t>
+  </si>
+  <si>
+    <t>Uno:</t>
+  </si>
+  <si>
+    <t>INH</t>
+  </si>
+  <si>
+    <t>DIR</t>
+  </si>
+  <si>
+    <t>EXT</t>
+  </si>
+  <si>
+    <t>IMM</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>IDX (5b)</t>
+  </si>
+  <si>
+    <t>IDX1</t>
+  </si>
+  <si>
+    <t>IDX2</t>
+  </si>
+  <si>
+    <t>IDX (pre-inc)</t>
+  </si>
+  <si>
+    <t>IDX (acc)</t>
+  </si>
+  <si>
+    <t>[IDX2]</t>
+  </si>
+  <si>
+    <t>[D,IDX]</t>
+  </si>
+  <si>
+    <t>REL (8b)</t>
+  </si>
+  <si>
+    <t>REL (16b)</t>
+  </si>
+  <si>
+    <t>REL (9b)</t>
+  </si>
+  <si>
+    <t>1 byte</t>
+  </si>
+  <si>
+    <t>2 byte</t>
+  </si>
+  <si>
+    <t>3 byte</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 byte</t>
+  </si>
+  <si>
+    <t>4 byte</t>
   </si>
 </sst>
 </file>
@@ -61,10 +207,18 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,7 +244,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -126,18 +280,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,215 +691,414 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>4040</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1" t="s">
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>300</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="1"/>
+      <c r="E26" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{409967B9-13A0-4814-8266-E35D35AAA4B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>